<commit_message>
prace na katalogu, pokusy upravovat vba pres python
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -618,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -686,6 +686,23 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bez jmena a hesla</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>\\192.168.000.000\</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
mnoho oprav v TRIMAZKONU
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -423,7 +423,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.000.255</t>
+          <t>192.168.10.255</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -448,7 +448,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>192.168.18.241</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -461,7 +461,7 @@
           <t>gggg</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>192.168.000.000g</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -486,7 +486,7 @@
           <t>du hast einen problem</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -560,12 +560,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>einkaufenfh</t>
+          <t>514</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>192.168.14.241</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>gggg</t>
+          <t xml:space="preserve">joo				</t>
         </is>
       </c>
       <c r="E1" t="n">
@@ -585,12 +585,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>einkaufenfh</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.14.241</t>
+          <t>192.168.18.241</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -600,7 +600,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">joo				</t>
+          <t>gggg</t>
         </is>
       </c>
       <c r="E2" t="n">

</xml_diff>

<commit_message>
ip adresa lze měnit bez admina pouze u připojených zařízení
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -436,8 +436,8 @@
           <t>kkgg</t>
         </is>
       </c>
-      <c r="E1" t="b">
-        <v>0</v>
+      <c r="E1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -574,7 +574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -632,6 +632,31 @@
         </is>
       </c>
       <c r="E2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>kartoffelnsalat</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.10.241</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>kkgg</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nova verze 3.6.2, funkcni interfaces, sledovani druhe adresy INET
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -804,7 +804,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ethernet,Ethernet 1,Ethernet 2,Ethernet 3,Ethernet 4,Ethernet 5,Wi-Fi,</t>
+          <t>Ethernet,Ethernet 3,WiFi,</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
vydani verze 3.7.0, plne funkcni ip manager, nova vizualizace menu
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6015" yWindow="1965" windowWidth="28800" windowHeight="15885" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="14940" yWindow="2640" windowWidth="23010" windowHeight="13650" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -404,10 +404,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -418,12 +418,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>kartoffelnsalat</t>
+          <t>fff</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.10.241</t>
+          <t>192.168.10.240</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -431,135 +431,7 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>kkgg</t>
-        </is>
-      </c>
-      <c r="E1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>einkaufenfh</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>192.168.18.241</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>gggg</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>bewolktt</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.000.000g</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>du hast einen problem
-d
-d
-d</t>
-        </is>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>514</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>192.168.14.241</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">joo				</t>
-        </is>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>regenschrim</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>fff</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>192.168.100.241</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>gf</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
+      <c r="E1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -574,93 +446,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A3" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.5703125" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>514</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>192.168.14.241</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">joo				</t>
-        </is>
-      </c>
-      <c r="E1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>einkaufenfh</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>192.168.18.241</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>gggg</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>kartoffelnsalat</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.10.241</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>kkgg</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -673,8 +469,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -756,6 +552,15 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>\\192.168.000.000\</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>a
+a
+a
+a
+aa</t>
         </is>
       </c>
     </row>
@@ -776,7 +581,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -793,7 +598,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
oprava, chyb, nové chyb hlášky
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3690" yWindow="5535" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10500" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -404,13 +404,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="20" customWidth="1" min="3" max="3"/>
   </cols>
@@ -437,6 +437,31 @@
         </is>
       </c>
       <c r="E1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>518</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.1.241</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>pozngg</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -457,9 +482,9 @@
       <selection activeCell="A3" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="15.5703125" customWidth="1" min="3" max="3"/>
+    <col width="15.5546875" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -472,22 +497,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="8.42578125" customWidth="1" min="2" max="2"/>
+    <col width="8.44140625" customWidth="1" min="2" max="2"/>
     <col width="32" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>518-2</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -497,7 +522,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>\\192.168.208.200\10_vision</t>
+          <t>\\192.168.208.200</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -557,6 +582,38 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>\\192.168.000.000\</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>518</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>druhá síť Valeo</t>
         </is>
       </c>
     </row>
@@ -578,13 +635,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="48.5703125" customWidth="1" min="1" max="1"/>
-    <col width="71.7109375" customWidth="1" min="2" max="2"/>
+    <col width="48.5546875" customWidth="1" min="1" max="1"/>
+    <col width="71.6640625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -616,7 +673,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -626,7 +683,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -642,11 +699,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>aktualizovat statusy disku default</t>
+          <t>aktualizovat statusy disku (default)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oprava duplikatu jmen, seznam online interfaces, DHCP, edit/needit pozn
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -476,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A1:E3"/>
@@ -486,7 +486,33 @@
   <cols>
     <col width="15.5546875" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>518</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>192.168.1.241</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pozngg</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
opravy v ip setting
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -433,7 +433,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>pozn</t>
+          <t>poznvv</t>
         </is>
       </c>
       <c r="E1" t="b">
@@ -458,10 +458,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>pozngg</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+          <t>poznggv
+df
+df
+df</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -505,7 +508,10 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>pozngg</t>
+          <t>poznggv
+df
+df
+df</t>
         </is>
       </c>
       <c r="E1" t="n">
@@ -658,7 +664,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -677,7 +683,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
@@ -729,7 +735,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>editovatelné(1)/ needitovatelné(0) poznámky (default)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ip setting - dhcp, nastavení chování mapování, catalogue maker - návod na přidělení práv makrům
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -684,7 +684,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -703,7 +703,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -735,7 +735,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -765,6 +765,16 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>disk persistentní - yes(1)/ no(0)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vylepseni v ip setting
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -404,7 +404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -418,12 +418,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>projekt</t>
+          <t>518</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.18.241</t>
+          <t>192.168.1.241</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -432,31 +432,6 @@
         </is>
       </c>
       <c r="D1" t="inlineStr">
-        <is>
-          <t>poznvv</t>
-        </is>
-      </c>
-      <c r="E1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>518</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>192.168.1.241</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
         <is>
           <t>poznggv
 df
@@ -464,27 +439,27 @@
 df</t>
         </is>
       </c>
+      <c r="E1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>514</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.14.241</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
       <c r="E2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>514</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.14.241</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -703,7 +678,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
zdařená optimalizace ip setting widgets, grid -> pack
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -434,9 +434,17 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>poznggv
-df
-df
-df</t>
+f
+fhk
+hvj
+hg
+guk
+f
+f
+f
+f
+jjjf
+f</t>
         </is>
       </c>
       <c r="E1" t="b">
@@ -457,6 +465,14 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>f
+f
+f
+f</t>
         </is>
       </c>
       <c r="E2" t="b">
@@ -660,7 +676,10 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>druhá síť Valeo</t>
+          <t>druhá síť Valeo
+fg
+f
+f</t>
         </is>
       </c>
     </row>
@@ -725,7 +744,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -747,7 +766,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -757,7 +776,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
nastavení catalogue ukládá do resources.txt
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -696,7 +696,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>\\10.9.250.100\</t>
+          <t>\\10.9.250.100</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
upraveni defaultnich cest, vizualizace ip setting, default cesta katalog, default nazev databaze
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10500" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -62,8 +62,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -404,26 +404,30 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
+    <col width="27.28515625" customWidth="1" min="1" max="1"/>
+    <col width="30.7109375" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="95.7109375" customWidth="1" min="4" max="4"/>
+    <col width="11.85546875" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>440_Austin</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.1.241</t>
+          <t>10.96.205.240</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -433,33 +437,27 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>poznggv
-f
-fhk
-hvj
-hg
-guk
-f
-f
-f
-f
-jjjf
-f</t>
+          <t>FortiClient Austin: 
+pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK
+FH-2050-20
+10.96.205.80</t>
         </is>
       </c>
       <c r="E1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>497_Edcha</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.14.241</t>
+          <t>172.26.7.240</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -469,25 +467,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>f
-f
-f
-f</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>515</t>
+          <t>503_Witte</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10.9.250.241</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -495,8 +490,254 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.205.267
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Teleflex </t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.14.240</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.???
+NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
+        </is>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.186</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Domaci Wifi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>474 B_Austin</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10.96.205.175</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.205.245
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>515_ZF Stara Boleslav</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10.9.250.240</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100
+User:spravce Pass:Jhv*2708 
+User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -510,26 +751,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15.5546875" customWidth="1" min="3" max="3"/>
+    <col width="15.5703125" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.1.241</t>
+          <t>192.168.1.243</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -537,15 +778,99 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>poznggv
-df
-df
-df</t>
-        </is>
-      </c>
       <c r="E1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.14.240</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.???
+NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>474 B_Austin</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10.96.205.175</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.205.245
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -560,98 +885,93 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="8.44140625" customWidth="1" min="2" max="2"/>
+    <col width="8.42578125" customWidth="1" min="2" max="2"/>
     <col width="32" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>518-2</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>\\192.168.208.200</t>
+          <t>\\192.168.14.245\Data\Kamery</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>jhv_vision</t>
+          <t>Vision</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>první sít, ixon</t>
+          <t>*Jhv2708</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>514-2</t>
+          <t>515_ZF</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>Z</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>jhvadmin</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>*Jhv2708</t>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>bez jmena a hesla</t>
+          <t>Domaci Nas</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>S</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.000.000\</t>
+          <t>\\192.168.1.20\Data</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -676,37 +996,75 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>druhá síť Valeo
-fg
-f
-f</t>
+          <t>Druha sít, ixon</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>515</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>\\10.9.250.100</t>
+          <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>spravce</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>474_B Austin</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\10.96.205.166\DATA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>10.96.205.166	
+VisionNas_474B	
+						user:JHV_Vision, omron 
+Pass:*Jhv2708</t>
         </is>
       </c>
     </row>
@@ -727,14 +1085,14 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="48.5546875" customWidth="1" min="1" max="1"/>
-    <col width="71.6640625" customWidth="1" min="2" max="2"/>
+    <col width="48.5703125" customWidth="1" min="1" max="1"/>
+    <col width="71.7109375" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -744,7 +1102,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
@@ -753,11 +1111,6 @@
           <t>list názvů rozhraní</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Ethernet,Ethernet 3,WiFi,</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -766,7 +1119,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -792,7 +1145,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>aktualizovat statusy disku (default)</t>
+          <t>aktualizovat statusy disků při vstupu do okna s disky (default)</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
release verze 3.7.6, úprava logiky poznámek v ip setting
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -437,12 +437,10 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>FortiClient Austin: 
-pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
-FH-2050-20
-10.96.205.80</t>
+          <t>FortiClient Austin: ajj
+adsfdd
+adf
+adf</t>
         </is>
       </c>
       <c r="E1" t="b">
@@ -492,18 +490,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.267
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
+          <t>PC:	10.96.205.175</t>
         </is>
       </c>
       <c r="E3" t="b">
@@ -554,11 +541,8 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
-CAM: 192.168.14.???
-NAS:192.168.14.245
-*******************************
-user: Vision
-pass: *Jhv2708</t>
+adf
+adf</t>
         </is>
       </c>
       <c r="E5" t="b">
@@ -668,18 +652,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.245
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
+          <t>PC:	10.96.205.175</t>
         </is>
       </c>
       <c r="E10" t="b">
@@ -705,7 +678,10 @@
       <c r="D11" t="inlineStr">
         <is>
           <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
+adf
+adf
+adf
+adf</t>
         </is>
       </c>
       <c r="E11" t="b">
@@ -730,10 +706,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>NAS - 10.9.250.100
-User:spravce Pass:Jhv*2708 
-User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
-123TPV456</t>
+          <t>NAS - 10.9.250.100</t>
         </is>
       </c>
       <c r="E12" t="b">
@@ -1119,7 +1092,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
uprava poznamek - enter prida radky, funkcni nova logika
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -437,10 +437,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>FortiClient Austin: ajj
-adsfdd
-adf
-adf</t>
+          <t>adfadf</t>
         </is>
       </c>
       <c r="E1" t="b">
@@ -465,7 +462,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
+          <t>FortiClient Edcha Ex2dp78kxp30
+sfg
+sffgs
+gsfg
+dfa
+f
+sfg
+sfg</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -490,7 +494,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.175</t>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.205.245
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK
+sf</t>
         </is>
       </c>
       <c r="E3" t="b">
@@ -515,7 +531,9 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Teleflex </t>
+          <t>Teleflex 
+sfg
+sgf</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -541,8 +559,8 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
-adf
-adf</t>
+f
+f</t>
         </is>
       </c>
       <c r="E5" t="b">
@@ -587,7 +605,8 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Kamera VS-S160MX :192.168.0.186</t>
+          <t>Kamera VS-S160MX :192.168.0.186
+ddfaajhdf</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -630,6 +649,11 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>afd</t>
+        </is>
+      </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
@@ -652,7 +676,8 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.175</t>
+          <t>PC:	10.96.205.175
+ajpodkjfa</t>
         </is>
       </c>
       <c r="E10" t="b">
@@ -678,9 +703,15 @@
       <c r="D11" t="inlineStr">
         <is>
           <t>XG-X2900:		10.101.28.175
+adfddd
+adfdddd
+adfdd
+adfg
+fg
+f
+df
 adf
-adf
-adf
+f
 adf</t>
         </is>
       </c>
@@ -1092,7 +1123,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
plne funkcni nova logika poznamek u ip, dodelat u disku, dodelat direct editing v oblíbených
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -437,7 +437,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>adfadf</t>
+          <t>FortiClient Austin: 
+pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK
+FH-2050-20
+10.96.205.80</t>
         </is>
       </c>
       <c r="E1" t="b">
@@ -462,14 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>FortiClient Edcha Ex2dp78kxp30
-sfg
-sffgs
-gsfg
-dfa
-f
-sfg
-sfg</t>
+          <t>FortiClient Edcha Ex2p78kxp30</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -493,6 +491,182 @@
         </is>
       </c>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.205.267
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Teleflex </t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.14.240</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.???
+NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
+        </is>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.186</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Domaci Wifi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>474 B_Austin</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10.96.205.175</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -505,179 +679,7 @@
 FortiClient Austin: 
 Pass:
 1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
-sf</t>
-        </is>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>511_Teleflex</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>192.168.1.242</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Teleflex 
-sfg
-sgf</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>514_Teleflex</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.14.240</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>PC:192.168.14.240
-f
-f</t>
-        </is>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>518_Valeo</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>192.168.208.242</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>529_Witte</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Kamera VS-S160MX :192.168.0.186
-ddfaajhdf</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Domaci Wifi</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>192.168.1.131</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>afd</t>
-        </is>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>474 B_Austin</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>10.96.205.175</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>PC:	10.96.205.175
-ajpodkjfa</t>
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
       <c r="E10" t="b">
@@ -703,16 +705,7 @@
       <c r="D11" t="inlineStr">
         <is>
           <t>XG-X2900:		10.101.28.175
-adfddd
-adfdddd
-adfdd
-adfg
-fg
-f
-df
-adf
-f
-adf</t>
+OP:		10.101.28.117</t>
         </is>
       </c>
       <c r="E11" t="b">
@@ -737,7 +730,10 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>NAS - 10.9.250.100</t>
+          <t>NAS - 10.9.250.100
+User:spravce Pass:Jhv*2708 
+User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
+123TPV456</t>
         </is>
       </c>
       <c r="E12" t="b">
@@ -1106,7 +1102,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -1123,7 +1119,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1153,7 +1149,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
dodelana nova logika poznamek u disků, opraveno chybové hlášení
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -404,7 +404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
@@ -558,7 +558,11 @@
 NAS:192.168.14.245
 *******************************
 user: Vision
-pass: *Jhv2708</t>
+pass: *Jhv2708
+f
+ffg
+f
+f</t>
         </is>
       </c>
       <c r="E5" t="b">
@@ -712,34 +716,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>515_ZF Stara Boleslav</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>10.9.250.240</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>NAS - 10.9.250.100
-User:spravce Pass:Jhv*2708 
-User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
-123TPV456</t>
-        </is>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -751,7 +727,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -805,7 +781,11 @@
 NAS:192.168.14.245
 *******************************
 user: Vision
-pass: *Jhv2708</t>
+pass: *Jhv2708
+f
+ffg
+f
+f</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -815,12 +795,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>474 B_Austin</t>
+          <t>527_Teijin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10.96.205.175</t>
+          <t>10.101.28.176</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -829,48 +809,12 @@
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.245
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>XG-X2900:		10.101.28.175
 OP:		10.101.28.117</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="E3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -885,7 +829,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -967,6 +911,12 @@
           <t>\\192.168.1.20\Data</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>f
+ffffffffffffffffff</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -996,14 +946,21 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Druha sít, ixon</t>
+          <t>Druha sít, ixonah
+dasf
+dfa
+dfa
+dfadfaafd
+daf
+dfa
+dfa</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>518_Valeo II8</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1013,7 +970,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>\\192.168.208.200\10_vision</t>
+          <t>\\192.168.1.10\10_vision</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1028,43 +985,14 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>474_B Austin</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\10.96.205.166\DATA</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>10.96.205.166	
-VisionNas_474B	
-						user:JHV_Vision, omron 
-Pass:*Jhv2708</t>
+          <t>Druha sít, ixonah
+dasf
+dfa
+dfa
+dfadfaafd
+daf
+dfa
+dfa</t>
         </is>
       </c>
     </row>
@@ -1102,7 +1030,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
prace na direct editing
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -437,12 +437,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>FortiClient Austin: 
-pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
-FH-2050-20
-10.96.205.80</t>
+          <t xml:space="preserve">FortiClient Austin: </t>
         </is>
       </c>
       <c r="E1" t="b">
@@ -492,18 +487,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.267
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
+          <t>PC:	10.96.205.175</t>
         </is>
       </c>
       <c r="E3" t="b">
@@ -553,16 +537,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PC:192.168.14.240
-CAM: 192.168.14.???
-NAS:192.168.14.245
-*******************************
-user: Vision
-pass: *Jhv2708
-f
-ffg
-f
-f</t>
+          <t>PC:192.168.14.240</t>
         </is>
       </c>
       <c r="E5" t="b">
@@ -648,6 +623,11 @@
       <c r="C9" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>saggggggggggf</t>
         </is>
       </c>
       <c r="E9" t="b">
@@ -693,12 +673,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>527_Teijin</t>
+          <t>527_Tei</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10.101.28.176</t>
+          <t>10.101.28.17</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -709,7 +689,7 @@
       <c r="D11" t="inlineStr">
         <is>
           <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
+OP:		10.101.28.</t>
         </is>
       </c>
       <c r="E11" t="b">
@@ -727,7 +707,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -754,19 +734,24 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E1" t="n">
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>saggggggggggf</t>
+        </is>
+      </c>
+      <c r="E1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>527_Tei</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.14.240</t>
+          <t>10.101.28.17</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -776,45 +761,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PC:192.168.14.240
-CAM: 192.168.14.???
-NAS:192.168.14.245
-*******************************
-user: Vision
-pass: *Jhv2708
-f
-ffg
-f
-f</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
           <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+OP:		10.101.28.</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -913,8 +864,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>f
-ffffffffffffffffff</t>
+          <t>f</t>
         </is>
       </c>
     </row>
@@ -946,14 +896,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Druha sít, ixonah
-dasf
-dfa
-dfa
-dfadfaafd
-daf
-dfa
-dfa</t>
+          <t>Druha sít, ixonah</t>
         </is>
       </c>
     </row>
@@ -985,14 +928,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Druha sít, ixonah
-dasf
-dfa
-dfa
-dfadfaafd
-daf
-dfa
-dfa</t>
+          <t>Druha sít, ixonah</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
plne funkcni direct editing
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9705" yWindow="4110" windowWidth="28695" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -62,8 +62,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
-    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -404,10 +404,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -422,12 +422,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>440_Austin</t>
+          <t>ggfs</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>10.96.205.240</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -437,22 +437,22 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t xml:space="preserve">FortiClient Austin: </t>
+          <t>ggiif</t>
         </is>
       </c>
       <c r="E1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>497_Edcha</t>
+          <t>518_Valeoo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>172.26.7.240</t>
+          <t>192.168.208.242</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -462,22 +462,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>503_Witte</t>
+          <t>oo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -487,22 +487,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.175</t>
+          <t>ooo</t>
         </is>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>511_Teleflex</t>
+          <t>527_Teihg</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.1.242</t>
+          <t>10.101.28.17</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -512,22 +512,23 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Teleflex </t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.h</t>
+        </is>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>kkkk</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.14.240</t>
+          <t>10.96.205.17</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -537,7 +538,9 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PC:192.168.14.240</t>
+          <t>PC:	10.96.205.175NAS:	10.96.205.166k
+FH:	10.96.205.154
+	10.96.20aa</t>
         </is>
       </c>
       <c r="E5" t="b">
@@ -547,12 +550,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>hhggg</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>192.168.208.242</t>
+          <t>192.168.000.000h</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -560,19 +563,24 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>hhh</t>
+        </is>
+      </c>
+      <c r="E6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>529_Witte</t>
+          <t>527_Tei</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>10.101.28.17</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -582,22 +590,23 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Kamera VS-S160MX :192.168.0.186</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.h</t>
+        </is>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Domaci Wifi</t>
+          <t>se</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>192.168.1.131</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -605,19 +614,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>h</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>192.168.1.243</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -625,24 +634,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>saggggggggggf</t>
-        </is>
-      </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>474 B_Austin</t>
+          <t>gg</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>10.96.205.175</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -650,35 +654,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.245
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
-        </is>
-      </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>527_Tei</t>
+          <t>jjs</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10.101.28.17</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -688,11 +676,90 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.</t>
+          <t>ss</t>
         </is>
       </c>
       <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>hhh</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>jjjj</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>aauj</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -707,10 +774,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C26" sqref="A8:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -721,12 +788,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>kkkk</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.1.243</t>
+          <t>10.96.205.17</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -736,22 +803,24 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>saggggggggggf</t>
-        </is>
-      </c>
-      <c r="E1" t="b">
+          <t>PC:	10.96.205.175NAS:	10.96.205.166k
+FH:	10.96.205.154
+	10.96.20aa</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>527_Tei</t>
+          <t>sssssssss</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10.101.28.17</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -759,13 +828,112 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sssse</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>aaaee</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>aauj</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>jjs</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1013,7 +1181,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
nová logika řazení editovaných projektů
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -404,7 +404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
@@ -422,12 +422,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ggfs</t>
+          <t>kkkk</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>10.96.205.17</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -436,113 +436,107 @@
         </is>
       </c>
       <c r="D1" t="inlineStr">
-        <is>
-          <t>ggiif</t>
-        </is>
-      </c>
-      <c r="E1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>518_Valeoo</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>192.168.208.242</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>oo</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ooo</t>
-        </is>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>527_Teihg</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10.101.28.17</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.h</t>
-        </is>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>kkkk</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>10.96.205.17</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175NAS:	10.96.205.166k
 FH:	10.96.205.154
 	10.96.20aa</t>
         </is>
       </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>jjjjb</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>jh</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>hhhd</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>axggg</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.000.000xg</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>axg</t>
+        </is>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>hhgggg</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.000.000h</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>hhh</t>
+        </is>
+      </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
@@ -550,12 +544,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>hhggg</t>
+          <t>jjs</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>192.168.000.000h</t>
+          <t>192.168.000.000j</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -565,22 +559,22 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>hhh</t>
+          <t>ssjdg</t>
         </is>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>527_Tei</t>
+          <t>sega</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10.101.28.17</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -590,18 +584,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.h</t>
+          <t>g</t>
         </is>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>se</t>
+          <t>aaujxa</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -614,19 +607,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E8" t="b">
-        <v>0</v>
+      <c r="E8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>ggzagga</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>192.168.000.0g</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -634,14 +627,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
       <c r="E9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>gg</t>
+          <t>haxs</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -654,112 +652,12 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>jjs</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>hhh</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>jjjj</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>aauj</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -774,7 +672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="A8:C26"/>
@@ -788,12 +686,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>kkkk</t>
+          <t>axggg</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>10.96.205.17</t>
+          <t>192.168.000.000xg</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -803,24 +701,22 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.175NAS:	10.96.205.166k
-FH:	10.96.205.154
-	10.96.20aa</t>
-        </is>
-      </c>
-      <c r="E1" t="n">
+          <t>axg</t>
+        </is>
+      </c>
+      <c r="E1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sssssssss</t>
+          <t>hhgggg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>192.168.000.000h</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -828,19 +724,24 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>hhh</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sssse</t>
+          <t>jjs</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>192.168.000.000j</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -848,14 +749,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ssjdg</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>aaaee</t>
+          <t>aaujxa</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -875,12 +781,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>aauj</t>
+          <t>ggzagga</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>192.168.000.0g</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -888,14 +794,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>gg</t>
+        </is>
+      </c>
+      <c r="E5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>jjs</t>
+          <t>haxs</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -910,30 +821,10 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1115,7 +1006,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1151,7 +1042,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1201,7 +1092,12 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
přepínání projektů v editu
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -704,8 +704,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
+          <t>XG-X2900:		10.101.28.175</t>
         </is>
       </c>
       <c r="E11" t="b">
@@ -866,8 +865,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
+          <t>XG-X2900:		10.101.28.175</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -1083,7 +1081,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1119,7 +1117,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1149,7 +1147,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1170,6 +1168,16 @@
       </c>
       <c r="B8" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>automaticky přesouvat upravené projekty na začátek</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vylepšování okna editu - ještě chyby při ukládání změn
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -404,7 +404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
@@ -513,12 +513,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>511_Teleflex</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.1.242</t>
+          <t>192.168.14.240</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -528,22 +528,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Teleflex </t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
+          <t>PC:192.168.14.240</t>
+        </is>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.14.240</t>
+          <t>192.168.208.242</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -551,29 +551,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>PC:192.168.14.240
-CAM: 192.168.14.???
-NAS:192.168.14.245
-*******************************
-user: Vision
-pass: *Jhv2708</t>
-        </is>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
+      <c r="E5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>527_Teijin</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>192.168.208.242</t>
+          <t>10.101.28.176</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -581,19 +571,24 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>0</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175</t>
+        </is>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>529_Witte</t>
+          <t>515_ZF Stara Boleslav</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>10.9.250.240</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -603,7 +598,10 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Kamera VS-S160MX :192.168.0.186</t>
+          <t>NAS - 10.9.250.100
+User:spravce Pass:Jhv*2708 
+User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
+123TPV456</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -613,12 +611,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Domaci Wifi</t>
+          <t>503_Witte</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>192.168.1.131</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -626,52 +624,12 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>474 B_Austin</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>10.96.205.175</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
 FH:	10.96.205.154
-	10.96.205.245
+	10.96.205.267
 -----------------------------------------
 user:JHV_Vision, omron 
 Pass:*Jhv2708
@@ -682,61 +640,8 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E10" t="b">
+      <c r="E8" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175</t>
-        </is>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>515_ZF Stara Boleslav</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>10.9.250.240</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>NAS - 10.9.250.100
-User:spravce Pass:Jhv*2708 
-User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
-123TPV456</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -750,7 +655,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -764,17 +669,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.1.243</t>
+          <t>192.168.14.240</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>PC:192.168.14.240</t>
         </is>
       </c>
       <c r="E1" t="n">
@@ -784,12 +694,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>527_Teijin</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.14.240</t>
+          <t>10.101.28.176</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -799,12 +709,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PC:192.168.14.240
-CAM: 192.168.14.???
-NAS:192.168.14.245
-*******************************
-user: Vision
-pass: *Jhv2708</t>
+          <t>XG-X2900:		10.101.28.175</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -814,12 +719,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>474 B_Austin</t>
+          <t>503_Witte</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10.96.205.175</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -832,7 +737,7 @@
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
 FH:	10.96.205.154
-	10.96.205.245
+	10.96.205.267
 -----------------------------------------
 user:JHV_Vision, omron 
 Pass:*Jhv2708
@@ -844,31 +749,6 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1100,7 +980,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -1117,7 +997,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
ukladání odvoleb mazani, funkcni bin složka při mazání
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9705" yWindow="4110" windowWidth="28695" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7380" yWindow="4665" windowWidth="28695" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="ip_adress_fav_list" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="disk_list" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Settings" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="projects_bin2" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -404,10 +405,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -422,12 +423,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>440_Austin</t>
+          <t>497_Edcha</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>10.96.205.240</t>
+          <t>172.26.7.240</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -437,27 +438,22 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>FortiClient Austin: 
-pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
-FH-2050-20
-10.96.205.80</t>
-        </is>
-      </c>
-      <c r="E1" t="b">
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>497_Edcha</t>
+          <t>503_Witte</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>172.26.7.240</t>
+          <t>192.168.0.240</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,31 +462,6 @@
         </is>
       </c>
       <c r="D2" t="inlineStr">
-        <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>503_Witte</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -506,29 +477,44 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E3" t="b">
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.14.240</t>
+          <t>192.168.1.243</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>PC:192.168.14.240</t>
         </is>
       </c>
       <c r="E4" t="b">
@@ -538,17 +524,23 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>527_Teijin</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.208.242</t>
+          <t>10.101.28.176</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -558,12 +550,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>527_Teijin</t>
+          <t>511_Teleflex</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10.101.28.176</t>
+          <t>192.168.1.242</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -573,75 +565,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28.175</t>
-        </is>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>515_ZF Stara Boleslav</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>10.9.250.240</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NAS - 10.9.250.100
-User:spravce Pass:Jhv*2708 
-User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
-123TPV456</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
+          <t xml:space="preserve">Teleflex </t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>503_Witte</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.267
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -669,12 +597,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.14.240</t>
+          <t>192.168.1.243</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -682,73 +610,7 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>PC:192.168.14.240</t>
-        </is>
-      </c>
       <c r="E1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>503_Witte</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.267
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -763,7 +625,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -805,144 +667,95 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>515_ZF</t>
+          <t>518_Valeo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+          <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>jhvadmin</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>jhvadm1n</t>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Domaci Nas</t>
+          <t>474_B Austin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.1.20\Data</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>\\192.168.1.10\10_vision</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+          <t>\\10.96.205.166\DATA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>518_Valeo</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>474_B Austin</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\10.96.205.166\DATA</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>10.96.205.166	
 VisionNas_474B	
 						user:JHV_Vision, omron 
 Pass:*Jhv2708</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>515_ZF</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jhvadmin</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>
@@ -961,9 +774,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1027,7 +840,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1047,7 +860,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -1058,9 +871,37 @@
       </c>
       <c r="B9" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>statusy odvolby dotazování při mazání</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
plne funkcni multi mazani controlem u ip adres
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7380" yWindow="4665" windowWidth="28695" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2130" yWindow="3930" windowWidth="28695" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -405,10 +405,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -423,12 +423,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>497_Edcha</t>
+          <t>440_Austin</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>172.26.7.240</t>
+          <t>10.96.205.240</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -438,7 +438,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
+          <t>FortiClient Austin: 
+pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK
+FH-2050-20
+10.96.205.80</t>
         </is>
       </c>
       <c r="E1" t="n">
@@ -448,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>503_Witte</t>
+          <t>497_Edcha</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>172.26.7.240</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -463,38 +468,32 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PC:	10.96.205.175
-NAS:	10.96.205.166
-FH:	10.96.205.154
-	10.96.205.267
------------------------------------------
-user:JHV_Vision, omron 
-Pass:*Jhv2708
----------------------------------------
-FortiClient Austin: 
-Pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>511_Teleflex</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.208.242</t>
+          <t>192.168.1.242</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Teleflex </t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -504,12 +503,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>Domaci Wifi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.1.243</t>
+          <t>192.168.1.131</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,19 +516,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E4" t="b">
-        <v>1</v>
+      <c r="E4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>527_Teijin</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10.101.28.176</t>
+          <t>192.168.14.240</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -539,36 +538,15 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.???
+NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>511_Teleflex</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>192.168.1.242</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Teleflex </t>
-        </is>
-      </c>
-      <c r="E6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -583,7 +561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -593,28 +571,7 @@
   <cols>
     <col width="15.5703125" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -625,7 +582,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -667,63 +624,89 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>518_Valeo</t>
+          <t>515_ZF</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>Z</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\192.168.208.200\10_vision</t>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>jhv_vision</t>
+          <t>jhvadmin</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>474_B Austin</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>10.96.205.166	
 VisionNas_474B	
@@ -732,30 +715,53 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>515_ZF</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>jhvadmin</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>jhvadm1n</t>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>první sít, ixon
+\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Domaci Nas</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>\\192.168.1.20\Data</t>
         </is>
       </c>
     </row>
@@ -793,7 +799,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -810,7 +816,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -820,7 +826,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -880,7 +886,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prace na vraceni zmen, oprava corrupted obrazku v prohlizeci
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -423,12 +423,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>440_Austin</t>
+          <t>514_Teleflexgg</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>10.96.205.240</t>
+          <t>192.168.14.240a</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -438,12 +438,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>FortiClient Austin: 
-pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
-FH-2050-20
-10.96.205.80</t>
+          <t>PC:192.168.14.240d</t>
         </is>
       </c>
       <c r="E1" t="n">
@@ -453,12 +448,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>497_Edcha</t>
+          <t>Df gga</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>172.26.7.240</t>
+          <t>192.168.1.131g</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,24 +461,19 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
+      <c r="E2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>511_Teleflex</t>
+          <t>Domaci Wifiaffz</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.1.242</t>
+          <t>192.168.1.13¨ks</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -493,60 +483,10 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Teleflex </t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Domaci Wifi</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>192.168.1.131</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>514_Teleflex</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.14.240</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>PC:192.168.14.240
-CAM: 192.168.14.???
-NAS:192.168.14.245
-*******************************
-user: Vision
-pass: *Jhv2708</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
+          <t>ddassssaa</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -561,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -571,18 +511,59 @@
   <cols>
     <col width="15.5703125" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Df gg</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>192.168.1.131g</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Df gga</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.1.131g</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -597,108 +578,98 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>515_ZF</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>jhvadmin</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>*Jhv2708</t>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>515_ZF</t>
+          <t>518_Valeo II</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
+          <t>\\192.168.1.10\10_vision</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>jhvadmin</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>jhvadm1n</t>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>Domaci Nas</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>S</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.1.10\10_vision</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon</t>
+          <t>\\192.168.1.20\Data</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>474_B Austin</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>\\10.96.205.166\DATA</t>
+          <t>\\192.168.14.245\Data\Kamery</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>jhv_vision</t>
+          <t>Vision</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -706,69 +677,8 @@
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>10.96.205.166	
-VisionNas_474B	
-						user:JHV_Vision, omron 
-Pass:*Jhv2708</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>518_Valeo</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>V</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>první sít, ixon
-\\192.168.208.200\10_vision</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Domaci Nas</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>\\192.168.1.20\Data</t>
-        </is>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
@@ -799,7 +709,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
@@ -816,7 +726,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -826,7 +736,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -900,14 +810,35 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Df  fsifa</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>192.168.1.131g</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload funkcniho vraceni změn
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2130" yWindow="3930" windowWidth="28695" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-21528" yWindow="2424" windowWidth="21624" windowHeight="11256" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="ip_adress_fav_list" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="disk_list" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Settings" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="projects_bin2" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="projects_bin2" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -20,20 +20,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -54,17 +46,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -423,12 +412,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>514_Teleflexgg</t>
+          <t>aaaaaaaa</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.14.240a</t>
+          <t>192.168.1.131</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -438,7 +427,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>PC:192.168.14.240d</t>
+          <t>ccxxxggd</t>
         </is>
       </c>
       <c r="E1" t="n">
@@ -448,12 +437,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Df gga</t>
+          <t>Domaci Wifiaffz</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.1.131g</t>
+          <t>192.168.1.13¨ks</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -461,19 +450,24 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ddassssaa</t>
+        </is>
+      </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Domaci Wifiaffz</t>
+          <t>514nnnzzzzz</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.1.13¨ks</t>
+          <t>192.168.14.240a</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -481,13 +475,8 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ddassssaa</t>
-        </is>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
+      <c r="E3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -515,12 +504,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Df gg</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.1.131g</t>
+          <t>192.168.14.240a</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -535,12 +524,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Df gga</t>
+          <t>514nnnzzzzz</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.1.131g</t>
+          <t>192.168.14.240a</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -548,7 +537,7 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E2" t="b">
+      <c r="E2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -692,7 +681,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -810,31 +799,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A2:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Df  fsifa</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>192.168.1.131g</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Domaci Wifiaffz</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.1.13¨ks</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E1" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ddassssaa</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nová logika zoomování, funkční malování
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -914,7 +914,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
@@ -1094,6 +1094,28 @@
 VisionNas_474B	
 						user:JHV_Vision, omron 
 Pass:*Jhv2708</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>xfdx</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>\\192.168.000.000\</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ss</t>
         </is>
       </c>
     </row>
@@ -1148,7 +1170,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1158,7 +1180,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
plne funkcni moznosti malovani v prohlizeci obrazku
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -1180,7 +1180,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
dodelani prohlizece, drobnosti v ip setting, pokusy komunikace s jiz spustenou aplikaci
</commit_message>
<xml_diff>
--- a/TRIMAZKON/saved_addresses_2.xlsx
+++ b/TRIMAZKON/saved_addresses_2.xlsx
@@ -555,8 +555,7 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
-CAM: 192.168.14.???
-NAS:192.168.14.245
+CAM: 192.168.14.??NAS:192.168.14.245
 *******************************
 user: Vision
 pass: *Jhv2708</t>
@@ -731,9 +730,8 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>NAS - 10.9.250.100
-User:spravce Pass:Jhv*2708 
-User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
+          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
+User:jhvadmin Pass:jhvm1n &gt;&gt;&gt; na portu 8080. 
 123TPV456</t>
         </is>
       </c>
@@ -802,8 +800,7 @@
       <c r="D2" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
-CAM: 192.168.14.???
-NAS:192.168.14.245
+CAM: 192.168.14.??NAS:192.168.14.245
 *******************************
 user: Vision
 pass: *Jhv2708</t>
@@ -893,9 +890,8 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NAS - 10.9.250.100
-User:spravce Pass:Jhv*2708 
-User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
+          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
+User:jhvadmin Pass:jhvm1n &gt;&gt;&gt; na portu 8080. 
 123TPV456</t>
         </is>
       </c>
@@ -1170,7 +1166,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>